<commit_message>
added ALU back in
</commit_message>
<xml_diff>
--- a/docs/SPAM1-20200527.xlsx
+++ b/docs/SPAM1-20200527.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{22961577-B69F-4CC7-B4CC-559AB671C2A7}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6E4CC4E7-8EA8-4475-906C-36BB6EBFF602}"/>
   <bookViews>
-    <workbookView xWindow="-66" yWindow="-66" windowWidth="23172" windowHeight="13092" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
   <sheets>
     <sheet name="AVR Like 24bit" sheetId="8" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="191">
   <si>
     <t>PCLOin</t>
   </si>
@@ -480,18 +480,6 @@
     <t>AMODE</t>
   </si>
   <si>
-    <t>Register pair setting - not for now</t>
-  </si>
-  <si>
-    <t>Cannot do unless got IR</t>
-  </si>
-  <si>
-    <t>MAR ideal but unless we have IR the AMODE must be PC as we are reading the ROM at current PC, but this means I cannot write RAM usefully because RAM/ROM share address bus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If R/W RAM then use MAR </t>
-  </si>
-  <si>
     <t>Advance PC (suppressed if just loaded PC)</t>
   </si>
   <si>
@@ -622,12 +610,57 @@
   <si>
     <t>only put here if could be read</t>
   </si>
+  <si>
+    <t>TODO MODE REGL/R TO LO BYTE AND ALU TO MID BYTE SO THE BITS LINE UP NICER ON ROMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>INST</t>
+  </si>
+  <si>
+    <t>OP1</t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For op1/2 we need the BUSR to contain the value from the instruction so </t>
+  </si>
+  <si>
+    <t>alternatively, we add another option to allow BUSR=INSTRUCTION_REG</t>
+  </si>
+  <si>
+    <t>FIXME !!</t>
+  </si>
+  <si>
+    <t>either we make the AMODE=PC which is easy but means we can't write CONST direct to the ram because we can't use ROM[PC] and RAM[MAR] at same time</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>Writing ROM is noop / writing RAM is undefined outcome as it is combinatorial operation</t>
+  </si>
+  <si>
+    <t>Reading ROM and writing to RAM is illogical as we only have one address bus</t>
+  </si>
+  <si>
+    <t>ACCESSING ROM AND RAM IN THIS OP IS ILLOGICAL AS ADDRESS BUS WOULD BE USELESS TO ONE OR OTHER DEVICE</t>
+  </si>
+  <si>
+    <t>Reading ROM or RAM,  and then writing to RAM is illogical, or undefined respectively, as we only have one address bus</t>
+  </si>
+  <si>
+    <t>INSTREG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -656,8 +689,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -730,8 +770,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -739,11 +785,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -795,6 +921,18 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,23 +1252,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D511976-8110-451C-91FE-D28B0C914776}">
-  <dimension ref="A1:AH48"/>
+  <dimension ref="A1:AN48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.5234375" customWidth="1"/>
-    <col min="2" max="2" width="25.15625" customWidth="1"/>
-    <col min="3" max="5" width="6.26171875" customWidth="1"/>
-    <col min="6" max="26" width="5.47265625" customWidth="1"/>
-    <col min="27" max="28" width="2.15625" customWidth="1"/>
-    <col min="29" max="33" width="7.41796875" customWidth="1"/>
+    <col min="1" max="1" width="3.54296875" customWidth="1"/>
+    <col min="2" max="2" width="25.1796875" customWidth="1"/>
+    <col min="3" max="5" width="6.26953125" customWidth="1"/>
+    <col min="6" max="26" width="5.453125" customWidth="1"/>
+    <col min="27" max="28" width="2.1796875" customWidth="1"/>
+    <col min="29" max="34" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B1" s="8" t="s">
         <v>106</v>
       </c>
@@ -1154,7 +1292,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
       <c r="B2" s="8" t="s">
         <v>108</v>
       </c>
@@ -1177,7 +1315,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3"/>
       <c r="B3" s="8" t="s">
         <v>107</v>
@@ -1195,22 +1333,22 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="15" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="16" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="W3" s="17"/>
       <c r="X3" s="17"/>
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
       <c r="F4" s="20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G4" s="21"/>
       <c r="H4" s="20"/>
@@ -1234,8 +1372,17 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="18"/>
-    </row>
-    <row r="5" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC4" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+    </row>
+    <row r="5" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C5" s="10">
         <v>23</v>
       </c>
@@ -1309,7 +1456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B6" s="10"/>
       <c r="C6" s="25">
         <v>7</v>
@@ -1392,15 +1539,15 @@
       <c r="AE6" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AF6" s="9" t="s">
+      <c r="AG6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="AG6" s="9" t="s">
+      <c r="AH6" s="9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>0</v>
       </c>
       <c r="B7" t="s">
@@ -1431,28 +1578,28 @@
         <v>69</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="O7" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="P7" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="Q7" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="R7" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="U7" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="V7" s="17" t="s">
         <v>60</v>
@@ -1478,18 +1625,19 @@
       <c r="AE7" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="AF7" s="17" t="s">
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="AG7" t="s">
+      <c r="AH7" t="s">
         <v>19</v>
       </c>
-      <c r="AH7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
+      <c r="AI7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -1547,19 +1695,17 @@
         <v>126</v>
       </c>
       <c r="AE8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF8" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF8" s="28"/>
+      <c r="AG8" t="s">
         <v>135</v>
       </c>
-      <c r="AG8" t="s">
-        <v>59</v>
-      </c>
       <c r="AH8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A9" s="28">
         <v>2</v>
       </c>
@@ -1637,19 +1783,17 @@
       </c>
       <c r="AD9" s="28"/>
       <c r="AE9" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF9" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="AG9" s="28" t="s">
+      <c r="AH9" t="s">
         <v>19</v>
       </c>
-      <c r="AH9" s="28" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A10" s="28">
         <v>3</v>
       </c>
@@ -1683,26 +1827,27 @@
       <c r="AA10" s="28"/>
       <c r="AB10" s="28"/>
       <c r="AC10" s="32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AD10" s="28"/>
       <c r="AE10" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF10" s="28" t="s">
-        <v>172</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="AF10" s="28"/>
       <c r="AG10" s="28" t="s">
-        <v>172</v>
-      </c>
-      <c r="AH10" s="28"/>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
+        <v>168</v>
+      </c>
+      <c r="AH10" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="AI10" s="28"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
         <v>4</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>109</v>
@@ -1782,22 +1927,22 @@
       <c r="AE11" t="s">
         <v>39</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AG11" t="s">
         <v>135</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AH11" t="s">
         <v>138</v>
       </c>
-      <c r="AH11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>109</v>
@@ -1877,14 +2022,17 @@
       <c r="AE12" t="s">
         <v>18</v>
       </c>
-      <c r="AF12" t="s">
+      <c r="AG12" t="s">
         <v>135</v>
       </c>
-      <c r="AG12" t="s">
+      <c r="AH12" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI12" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1901,19 +2049,19 @@
         <v>109</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>72</v>
@@ -1967,44 +2115,48 @@
         <v>18</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>162</v>
-      </c>
+        <v>165</v>
+      </c>
+      <c r="AF13" s="7"/>
       <c r="AG13" t="s">
+        <v>158</v>
+      </c>
+      <c r="AH13" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="AI13" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9"/>
       <c r="AC14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AE14" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="AG14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+        <v>168</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -2015,19 +2167,19 @@
         <v>119</v>
       </c>
       <c r="AC16" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="AD16" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="AE16" t="s">
-        <v>174</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>170</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>0</v>
       </c>
@@ -2039,7 +2191,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2055,10 +2207,27 @@
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="Q18" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+        <v>169</v>
+      </c>
+      <c r="AB18" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="36"/>
+      <c r="AH18" s="36"/>
+      <c r="AI18" s="36"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="36"/>
+      <c r="AL18" s="36"/>
+      <c r="AM18" s="36"/>
+      <c r="AN18" s="37"/>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2087,8 +2256,29 @@
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="39"/>
+      <c r="AD19" s="39" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE19" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF19" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG19" s="39" t="s">
+        <v>184</v>
+      </c>
+      <c r="AH19" s="39"/>
+      <c r="AI19" s="39"/>
+      <c r="AJ19" s="39"/>
+      <c r="AK19" s="39"/>
+      <c r="AL19" s="39"/>
+      <c r="AM19" s="39"/>
+      <c r="AN19" s="41"/>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2116,8 +2306,29 @@
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="39"/>
+      <c r="AD20" s="39" t="s">
+        <v>180</v>
+      </c>
+      <c r="AE20" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF20" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG20" s="39" t="s">
+        <v>182</v>
+      </c>
+      <c r="AH20" s="39"/>
+      <c r="AI20" s="39"/>
+      <c r="AJ20" s="39"/>
+      <c r="AK20" s="39"/>
+      <c r="AL20" s="39"/>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="41"/>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2142,8 +2353,21 @@
       <c r="W21" s="12"/>
       <c r="X21" s="12"/>
       <c r="Y21" s="12"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="39"/>
+      <c r="AD21" s="39"/>
+      <c r="AE21" s="39"/>
+      <c r="AF21" s="39"/>
+      <c r="AG21" s="39"/>
+      <c r="AH21" s="39"/>
+      <c r="AI21" s="39"/>
+      <c r="AJ21" s="39"/>
+      <c r="AK21" s="39"/>
+      <c r="AL21" s="39"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="41"/>
+    </row>
+    <row r="22" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>5</v>
       </c>
@@ -2171,8 +2395,21 @@
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="AB22" s="42"/>
+      <c r="AC22" s="43"/>
+      <c r="AD22" s="43"/>
+      <c r="AE22" s="43"/>
+      <c r="AF22" s="43"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="43"/>
+      <c r="AI22" s="43"/>
+      <c r="AJ22" s="43"/>
+      <c r="AK22" s="43"/>
+      <c r="AL22" s="43"/>
+      <c r="AM22" s="43"/>
+      <c r="AN22" s="44"/>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
@@ -2186,7 +2423,7 @@
         <v>2</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="I23" s="1"/>
       <c r="L23" s="11"/>
@@ -2204,7 +2441,7 @@
       <c r="X23" s="12"/>
       <c r="Y23" s="13"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
@@ -2218,13 +2455,13 @@
         <v>3</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H24" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I24" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="K24" s="12"/>
       <c r="L24" s="11"/>
@@ -2241,7 +2478,7 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
@@ -2255,13 +2492,13 @@
         <v>4</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H25" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I25" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K25" s="12"/>
       <c r="L25" s="11"/>
@@ -2278,7 +2515,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
@@ -2292,10 +2529,10 @@
         <v>5</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H26" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -2312,7 +2549,7 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -2326,13 +2563,13 @@
         <v>6</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="K27" s="11"/>
       <c r="L27" s="12"/>
@@ -2349,7 +2586,7 @@
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11</v>
       </c>
@@ -2363,10 +2600,10 @@
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="I28" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
@@ -2383,7 +2620,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12</v>
       </c>
@@ -2410,7 +2647,7 @@
       <c r="V29" s="12"/>
       <c r="W29" s="12"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>13</v>
       </c>
@@ -2434,7 +2671,7 @@
       <c r="V30" s="12"/>
       <c r="W30" s="12"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>14</v>
       </c>
@@ -2442,13 +2679,13 @@
         <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I31" s="1"/>
       <c r="L31" s="11"/>
@@ -2464,7 +2701,7 @@
       <c r="V31" s="12"/>
       <c r="W31" s="12"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>15</v>
       </c>
@@ -2472,13 +2709,13 @@
         <v>110</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G32" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="I32" s="1"/>
       <c r="L32" s="12"/>
@@ -2494,7 +2731,7 @@
       <c r="V32" s="12"/>
       <c r="W32" s="12"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>16</v>
       </c>
@@ -2505,10 +2742,10 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G33" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I33" s="1"/>
       <c r="L33" s="12"/>
@@ -2524,7 +2761,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>17</v>
       </c>
@@ -2535,10 +2772,10 @@
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="I34" s="1"/>
       <c r="M34" s="12"/>
@@ -2553,7 +2790,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>18</v>
       </c>
@@ -2564,15 +2801,15 @@
         <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G35" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I35" s="1"/>
       <c r="L35" s="11"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>19</v>
       </c>
@@ -2584,7 +2821,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>20</v>
       </c>
@@ -2596,7 +2833,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>21</v>
       </c>
@@ -2608,7 +2845,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>22</v>
       </c>
@@ -2632,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>23</v>
       </c>
@@ -2656,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>24</v>
       </c>
@@ -2680,7 +2917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>25</v>
       </c>
@@ -2704,7 +2941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>26</v>
       </c>
@@ -2728,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>27</v>
       </c>
@@ -2752,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>28</v>
       </c>
@@ -2776,7 +3013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>29</v>
       </c>
@@ -2800,7 +3037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>30</v>
       </c>
@@ -2812,7 +3049,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>31</v>
       </c>
@@ -2839,14 +3076,14 @@
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="G5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
@@ -2860,7 +3097,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -2874,7 +3111,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2894,7 +3131,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2914,7 +3151,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -2934,7 +3171,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -2951,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +3205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
@@ -2985,7 +3222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
@@ -3002,7 +3239,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
@@ -3019,7 +3256,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
@@ -3036,7 +3273,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -3053,7 +3290,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
@@ -3067,7 +3304,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
@@ -3081,7 +3318,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
@@ -3098,7 +3335,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
@@ -3115,7 +3352,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
@@ -3132,7 +3369,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
@@ -3152,7 +3389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
@@ -3172,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
@@ -3192,7 +3429,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
@@ -3212,7 +3449,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
@@ -3232,7 +3469,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -3249,7 +3486,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
@@ -3266,7 +3503,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
@@ -3283,7 +3520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
@@ -3303,7 +3540,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
@@ -3323,7 +3560,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
@@ -3343,7 +3580,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -3363,7 +3600,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
@@ -3383,7 +3620,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
@@ -3403,7 +3640,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
@@ -3423,7 +3660,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
@@ -3457,17 +3694,17 @@
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.15625" customWidth="1"/>
-    <col min="10" max="10" width="8.7890625" customWidth="1"/>
+    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -3478,7 +3715,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3495,7 +3732,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0</v>
       </c>
@@ -3518,7 +3755,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -3541,7 +3778,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -3564,7 +3801,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3587,7 +3824,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0</v>
       </c>
@@ -3613,7 +3850,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3648,7 +3885,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -3680,7 +3917,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -3709,7 +3946,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3738,7 +3975,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -3767,7 +4004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -3796,7 +4033,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0</v>
       </c>
@@ -3825,7 +4062,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0</v>
       </c>
@@ -3851,7 +4088,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3874,7 +4111,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0</v>
       </c>
@@ -3897,7 +4134,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0</v>
       </c>
@@ -3920,7 +4157,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -3949,7 +4186,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -3975,7 +4212,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>1</v>
       </c>
@@ -4001,7 +4238,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>1</v>
       </c>
@@ -4027,7 +4264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>1</v>
       </c>
@@ -4053,7 +4290,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>1</v>
       </c>
@@ -4079,7 +4316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="5">
         <v>1</v>
       </c>
@@ -4105,7 +4342,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>1</v>
       </c>
@@ -4131,7 +4368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -4157,7 +4394,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>1</v>
       </c>
@@ -4183,7 +4420,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>1</v>
       </c>
@@ -4209,7 +4446,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>1</v>
       </c>
@@ -4235,7 +4472,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -4261,7 +4498,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>1</v>
       </c>
@@ -4287,7 +4524,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>1</v>
       </c>
@@ -4313,7 +4550,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
loop counter program working - found bug in reg file wiring that caused a loop that interfered in counting (clk needed to wire to exec and not to system clock) - however there are bugs due to ALU not using carry in so program OUGHT to fail but doesnt
</commit_message>
<xml_diff>
--- a/docs/SPAM1-20200527.xlsx
+++ b/docs/SPAM1-20200527.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="487" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE867CC6-E116-49AC-9C75-6EEC2AF3241E}"/>
+  <xr:revisionPtr revIDLastSave="537" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB99D2B7-C315-4314-94FD-F405196CA979}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="WriteDecoder" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="201">
   <si>
     <t>PCLOin</t>
   </si>
@@ -645,15 +646,6 @@
     <t>Addr</t>
   </si>
   <si>
-    <t>Adev</t>
-  </si>
-  <si>
-    <t>Tdev</t>
-  </si>
-  <si>
-    <t>Bdev</t>
-  </si>
-  <si>
     <t>AluOp</t>
   </si>
   <si>
@@ -670,6 +662,30 @@
   </si>
   <si>
     <t>Also ..</t>
+  </si>
+  <si>
+    <t>Dest</t>
+  </si>
+  <si>
+    <t>Asrc</t>
+  </si>
+  <si>
+    <t>Bsrc</t>
+  </si>
+  <si>
+    <t>Make every operations A = A ALU B</t>
+  </si>
+  <si>
+    <t>To make the RAM sync I'll need a data in register, and toggle the OE/WE on the execute phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map devices like UART/PC/MAR to specific addresses eg on page  ff so they are out of the way </t>
+  </si>
+  <si>
+    <t>ROM occupy lower 32 k and RAM the upper 32 k</t>
+  </si>
+  <si>
+    <t>Top bit of address will determine if A or B address goes on the Ram or Rom address bus</t>
   </si>
 </sst>
 </file>
@@ -866,7 +882,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -999,6 +1015,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1010,7 +1037,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1087,13 +1114,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="18" borderId="10" xfId="5"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="11" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1422,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436307F2-2BE4-4354-B58A-2AD970B44198}">
   <dimension ref="A1:XFD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17845,7 +17875,7 @@
         <v>4</v>
       </c>
       <c r="Z4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="AA4">
         <v>3</v>
@@ -18011,61 +18041,61 @@
         <v>93</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="L6" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="M6" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="N6" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="O6" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="P6" s="47" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q6" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="R6" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="S6" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="T6" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="U6" t="s">
         <v>190</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="I6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="J6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="K6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="L6" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="M6" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="N6" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="O6" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="P6" s="47" t="s">
-        <v>187</v>
-      </c>
-      <c r="Q6" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="R6" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="S6" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="T6" s="48" t="s">
-        <v>189</v>
-      </c>
-      <c r="U6" t="s">
-        <v>193</v>
       </c>
       <c r="X6" t="s">
         <v>7</v>
@@ -18074,79 +18104,79 @@
         <v>7</v>
       </c>
       <c r="Z6" s="49" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="AA6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP6" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AQ6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AB6" s="50" t="s">
+      <c r="AR6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AC6" s="50" t="s">
+      <c r="AS6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AD6" s="50" t="s">
+      <c r="AT6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AE6" s="50" t="s">
+      <c r="AU6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AF6" s="50" t="s">
+      <c r="AV6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AG6" s="50" t="s">
+      <c r="AW6" s="52" t="s">
         <v>185</v>
       </c>
-      <c r="AH6" s="50" t="s">
+      <c r="AX6" s="52" t="s">
         <v>185</v>
-      </c>
-      <c r="AI6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AJ6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AL6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AM6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AN6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AO6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AP6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AQ6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AR6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AS6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AT6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AU6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AV6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AW6" s="51" t="s">
-        <v>186</v>
-      </c>
-      <c r="AX6" s="51" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:16384" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -18171,31 +18201,31 @@
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
       <c r="AP7" t="s">
-        <v>195</v>
-      </c>
-      <c r="AQ7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AR7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AS7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AT7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AU7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AV7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AW7" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="AX7" s="52" t="s">
-        <v>194</v>
+        <v>192</v>
+      </c>
+      <c r="AQ7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AR7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AT7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AU7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AV7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AW7" s="51" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX7" s="51" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
@@ -18220,31 +18250,251 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
-      <c r="K9" s="29"/>
-      <c r="L9" s="29"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="29"/>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-      <c r="T9" s="29"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
+    <row r="9" spans="1:16384" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="45">
+        <v>7</v>
+      </c>
+      <c r="D9" s="45">
+        <v>6</v>
+      </c>
+      <c r="E9" s="45">
+        <v>5</v>
+      </c>
+      <c r="F9" s="45">
+        <v>4</v>
+      </c>
+      <c r="G9" s="45">
+        <v>3</v>
+      </c>
+      <c r="H9" s="45">
+        <v>2</v>
+      </c>
+      <c r="I9" s="45">
+        <v>1</v>
+      </c>
+      <c r="J9" s="45">
+        <v>0</v>
+      </c>
+      <c r="K9" s="25">
+        <v>7</v>
+      </c>
+      <c r="L9" s="25">
+        <v>6</v>
+      </c>
+      <c r="M9" s="25">
+        <v>5</v>
+      </c>
+      <c r="N9" s="25">
+        <v>4</v>
+      </c>
+      <c r="O9" s="25">
+        <v>3</v>
+      </c>
+      <c r="P9" s="25">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="25">
+        <v>1</v>
+      </c>
+      <c r="R9" s="25">
+        <v>0</v>
+      </c>
+      <c r="S9" s="45">
+        <v>7</v>
+      </c>
+      <c r="T9" s="45">
+        <v>6</v>
+      </c>
+      <c r="U9" s="45">
+        <v>5</v>
+      </c>
+      <c r="V9" s="45">
+        <v>4</v>
+      </c>
+      <c r="W9" s="45">
+        <v>3</v>
+      </c>
+      <c r="X9" s="45">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="45">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="45">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="25">
+        <v>7</v>
+      </c>
+      <c r="AB9" s="25">
+        <v>6</v>
+      </c>
+      <c r="AC9" s="25">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="25">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="25">
+        <v>3</v>
+      </c>
+      <c r="AF9" s="25">
+        <v>2</v>
+      </c>
+      <c r="AG9" s="25">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="25">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="45">
+        <v>7</v>
+      </c>
+      <c r="AJ9" s="45">
+        <v>6</v>
+      </c>
+      <c r="AK9" s="45">
+        <v>5</v>
+      </c>
+      <c r="AL9" s="45">
+        <v>4</v>
+      </c>
+      <c r="AM9" s="45">
+        <v>3</v>
+      </c>
+      <c r="AN9" s="45">
+        <v>2</v>
+      </c>
+      <c r="AO9" s="45">
+        <v>1</v>
+      </c>
+      <c r="AP9" s="45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16384" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="L10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="M10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="N10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="O10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="P10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="R10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="S10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="T10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="U10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="V10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="W10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="X10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z10" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="AA10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AB10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AE10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AF10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AG10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AI10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AJ10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AK10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AM10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AN10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AO10" s="50" t="s">
+        <v>186</v>
+      </c>
+      <c r="AP10" s="50" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16384" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -18255,7 +18505,9 @@
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
+      <c r="K11" s="12" t="s">
+        <v>198</v>
+      </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -18277,7 +18529,9 @@
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="K12" s="12" t="s">
+        <v>196</v>
+      </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -18297,9 +18551,10 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
       <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
+      <c r="K13" s="12" t="s">
+        <v>197</v>
+      </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -18314,6 +18569,9 @@
       <c r="W13" s="9"/>
     </row>
     <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
+      <c r="K14" s="53" t="s">
+        <v>199</v>
+      </c>
       <c r="AB14" s="1"/>
       <c r="AF14" s="12"/>
       <c r="AG14" s="11"/>
@@ -18331,6 +18589,9 @@
       <c r="AS14" s="12"/>
     </row>
     <row r="15" spans="1:16384" x14ac:dyDescent="0.35">
+      <c r="K15" s="53" t="s">
+        <v>200</v>
+      </c>
       <c r="AB15" s="1"/>
       <c r="AF15" s="12"/>
       <c r="AG15" s="11"/>

</xml_diff>

<commit_message>
alu code and rom version equate now
</commit_message>
<xml_diff>
--- a/docs/SPAM1-20200527.xlsx
+++ b/docs/SPAM1-20200527.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db8094ce4aaa691d/simplecpu/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="537" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EB99D2B7-C315-4314-94FD-F405196CA979}"/>
+  <xr:revisionPtr revIDLastSave="565" documentId="8_{481D5F51-72AF-42BD-AF55-70253197EE24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2FC7B993-C8C6-46A3-8921-2DE3C59F678A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
+    <workbookView xWindow="-66" yWindow="-66" windowWidth="23172" windowHeight="12492" xr2:uid="{B4484DA9-D572-4854-B84C-0917FAD72649}"/>
   </bookViews>
   <sheets>
     <sheet name="AVR Like 24bit WIDE" sheetId="10" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="WriteDecoder" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1452,31 +1451,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{436307F2-2BE4-4354-B58A-2AD970B44198}">
   <dimension ref="A1:XFD38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="F2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="46" width="6.26953125" customWidth="1"/>
-    <col min="47" max="67" width="5.453125" customWidth="1"/>
-    <col min="68" max="69" width="2.1796875" customWidth="1"/>
-    <col min="70" max="75" width="7.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.5234375" customWidth="1"/>
+    <col min="2" max="2" width="25.15625" customWidth="1"/>
+    <col min="3" max="46" width="6.26171875" customWidth="1"/>
+    <col min="47" max="67" width="5.47265625" customWidth="1"/>
+    <col min="68" max="69" width="2.15625" customWidth="1"/>
+    <col min="70" max="75" width="7.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:16384" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16384" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3"/>
       <c r="B3" s="8" t="s">
         <v>107</v>
@@ -17864,7 +17863,7 @@
       <c r="XFC3"/>
       <c r="XFD3"/>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="C4">
         <v>6</v>
       </c>
@@ -17887,7 +17886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16384" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C5" s="45">
         <v>7</v>
       </c>
@@ -18033,7 +18032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16384" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A6" s="1">
         <v>0</v>
       </c>
@@ -18179,7 +18178,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16384" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -18228,7 +18227,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="29"/>
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
@@ -18250,7 +18249,7 @@
       <c r="S8" s="29"/>
       <c r="T8" s="29"/>
     </row>
-    <row r="9" spans="1:16384" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16384" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="C9" s="45">
         <v>7</v>
       </c>
@@ -18372,7 +18371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16384" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16384" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -18494,7 +18493,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16384" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -18518,7 +18517,7 @@
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -18542,7 +18541,7 @@
       <c r="S12" s="9"/>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -18568,7 +18567,7 @@
       <c r="V13" s="9"/>
       <c r="W13" s="9"/>
     </row>
-    <row r="14" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="K14" s="53" t="s">
         <v>199</v>
       </c>
@@ -18588,7 +18587,7 @@
       <c r="AR14" s="12"/>
       <c r="AS14" s="12"/>
     </row>
-    <row r="15" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="K15" s="53" t="s">
         <v>200</v>
       </c>
@@ -18608,7 +18607,7 @@
       <c r="AR15" s="12"/>
       <c r="AS15" s="12"/>
     </row>
-    <row r="16" spans="1:16384" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.55000000000000004">
       <c r="AB16" s="1"/>
       <c r="AF16" s="12"/>
       <c r="AG16" s="12"/>
@@ -18625,7 +18624,7 @@
       <c r="AR16" s="12"/>
       <c r="AS16" s="12"/>
     </row>
-    <row r="17" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="17" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AB17" s="1"/>
       <c r="AF17" s="11"/>
       <c r="AG17" s="12"/>
@@ -18642,7 +18641,7 @@
       <c r="AR17" s="12"/>
       <c r="AS17" s="12"/>
     </row>
-    <row r="18" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="18" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AG18" s="12"/>
       <c r="AH18" s="12"/>
       <c r="AI18" s="12"/>
@@ -18658,7 +18657,7 @@
       <c r="AS18" s="12"/>
       <c r="AT18" s="12"/>
     </row>
-    <row r="19" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="19" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD19" s="1"/>
       <c r="AG19" s="12"/>
       <c r="AH19" s="12"/>
@@ -18673,7 +18672,7 @@
       <c r="AQ19" s="12"/>
       <c r="AR19" s="12"/>
     </row>
-    <row r="20" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="20" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD20" s="1"/>
       <c r="AG20" s="12"/>
       <c r="AH20" s="12"/>
@@ -18688,7 +18687,7 @@
       <c r="AQ20" s="12"/>
       <c r="AR20" s="12"/>
     </row>
-    <row r="21" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="21" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AA21" s="1"/>
       <c r="AD21" s="1"/>
       <c r="AG21" s="11"/>
@@ -18704,7 +18703,7 @@
       <c r="AQ21" s="12"/>
       <c r="AR21" s="12"/>
     </row>
-    <row r="22" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="22" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AA22" s="1"/>
       <c r="AD22" s="1"/>
       <c r="AG22" s="12"/>
@@ -18720,7 +18719,7 @@
       <c r="AQ22" s="12"/>
       <c r="AR22" s="12"/>
     </row>
-    <row r="23" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="23" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD23" s="1"/>
       <c r="AG23" s="12"/>
       <c r="AH23" s="12"/>
@@ -18735,7 +18734,7 @@
       <c r="AQ23" s="12"/>
       <c r="AR23" s="12"/>
     </row>
-    <row r="24" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="24" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD24" s="1"/>
       <c r="AH24" s="12"/>
       <c r="AI24" s="12"/>
@@ -18749,47 +18748,47 @@
       <c r="AQ24" s="12"/>
       <c r="AR24" s="12"/>
     </row>
-    <row r="25" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="25" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD25" s="1"/>
       <c r="AG25" s="11"/>
     </row>
-    <row r="26" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="26" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD26" s="1"/>
     </row>
-    <row r="27" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="27" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD27" s="1"/>
     </row>
-    <row r="28" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="28" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="29" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD29" s="1"/>
     </row>
-    <row r="30" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="30" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD30" s="1"/>
     </row>
-    <row r="31" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="31" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD31" s="1"/>
     </row>
-    <row r="32" spans="27:46" x14ac:dyDescent="0.35">
+    <row r="32" spans="27:46" x14ac:dyDescent="0.55000000000000004">
       <c r="AD32" s="1"/>
     </row>
-    <row r="33" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="33" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD33" s="1"/>
     </row>
-    <row r="34" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="34" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD34" s="1"/>
     </row>
-    <row r="35" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="35" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD35" s="1"/>
     </row>
-    <row r="36" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="36" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD36" s="1"/>
     </row>
-    <row r="37" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="37" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD37" s="1"/>
     </row>
-    <row r="38" spans="30:30" x14ac:dyDescent="0.35">
+    <row r="38" spans="30:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AD38" s="1"/>
     </row>
   </sheetData>
@@ -18806,17 +18805,17 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.54296875" customWidth="1"/>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="5" width="6.26953125" customWidth="1"/>
-    <col min="6" max="26" width="5.453125" customWidth="1"/>
-    <col min="27" max="28" width="2.1796875" customWidth="1"/>
-    <col min="29" max="34" width="7.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.5234375" customWidth="1"/>
+    <col min="2" max="2" width="25.15625" customWidth="1"/>
+    <col min="3" max="5" width="6.26171875" customWidth="1"/>
+    <col min="6" max="26" width="5.47265625" customWidth="1"/>
+    <col min="27" max="28" width="2.15625" customWidth="1"/>
+    <col min="29" max="34" width="7.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="8" t="s">
         <v>106</v>
       </c>
@@ -18840,7 +18839,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="8" t="s">
         <v>108</v>
       </c>
@@ -18863,7 +18862,7 @@
       <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
     </row>
-    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3"/>
       <c r="B3" s="8" t="s">
         <v>107</v>
@@ -18894,7 +18893,7 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="F4" s="20" t="s">
         <v>154</v>
       </c>
@@ -18930,7 +18929,7 @@
       <c r="AH4" s="34"/>
       <c r="AI4" s="34"/>
     </row>
-    <row r="5" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="10">
         <v>23</v>
       </c>
@@ -19004,7 +19003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="10"/>
       <c r="C6" s="25">
         <v>7</v>
@@ -19094,7 +19093,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -19184,7 +19183,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>1</v>
       </c>
@@ -19253,7 +19252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="28">
         <v>2</v>
       </c>
@@ -19341,7 +19340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="28">
         <v>3</v>
       </c>
@@ -19390,7 +19389,7 @@
       </c>
       <c r="AI10" s="28"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -19485,7 +19484,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>5</v>
       </c>
@@ -19580,7 +19579,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>6</v>
       </c>
@@ -19679,7 +19678,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>7</v>
       </c>
@@ -19702,12 +19701,12 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>136</v>
       </c>
@@ -19730,7 +19729,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:40" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A17">
         <v>0</v>
       </c>
@@ -19742,7 +19741,7 @@
       </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>1</v>
       </c>
@@ -19774,7 +19773,7 @@
       <c r="AM18" s="36"/>
       <c r="AN18" s="37"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>2</v>
       </c>
@@ -19821,7 +19820,7 @@
       <c r="AM19" s="39"/>
       <c r="AN19" s="41"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>3</v>
       </c>
@@ -19865,7 +19864,7 @@
       <c r="AM20" s="39"/>
       <c r="AN20" s="41"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>4</v>
       </c>
@@ -19906,7 +19905,7 @@
       <c r="AM21" s="39"/>
       <c r="AN21" s="41"/>
     </row>
-    <row r="22" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:40" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A22">
         <v>5</v>
       </c>
@@ -19948,7 +19947,7 @@
       <c r="AM22" s="43"/>
       <c r="AN22" s="44"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>6</v>
       </c>
@@ -19980,7 +19979,7 @@
       <c r="X23" s="12"/>
       <c r="Y23" s="13"/>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>7</v>
       </c>
@@ -20017,7 +20016,7 @@
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>8</v>
       </c>
@@ -20054,7 +20053,7 @@
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>9</v>
       </c>
@@ -20091,7 +20090,7 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>10</v>
       </c>
@@ -20123,7 +20122,7 @@
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>11</v>
       </c>
@@ -20151,7 +20150,7 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>12</v>
       </c>
@@ -20178,7 +20177,7 @@
       <c r="V29" s="12"/>
       <c r="W29" s="12"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <v>13</v>
       </c>
@@ -20202,7 +20201,7 @@
       <c r="V30" s="12"/>
       <c r="W30" s="12"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <v>14</v>
       </c>
@@ -20232,7 +20231,7 @@
       <c r="V31" s="12"/>
       <c r="W31" s="12"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <v>15</v>
       </c>
@@ -20262,7 +20261,7 @@
       <c r="V32" s="12"/>
       <c r="W32" s="12"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <v>16</v>
       </c>
@@ -20292,7 +20291,7 @@
       <c r="V33" s="12"/>
       <c r="W33" s="12"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <v>17</v>
       </c>
@@ -20321,7 +20320,7 @@
       <c r="V34" s="12"/>
       <c r="W34" s="12"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <v>18</v>
       </c>
@@ -20340,7 +20339,7 @@
       <c r="I35" s="1"/>
       <c r="L35" s="11"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <v>19</v>
       </c>
@@ -20352,7 +20351,7 @@
       </c>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <v>20</v>
       </c>
@@ -20364,7 +20363,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <v>21</v>
       </c>
@@ -20376,7 +20375,7 @@
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <v>22</v>
       </c>
@@ -20400,7 +20399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <v>23</v>
       </c>
@@ -20424,7 +20423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <v>24</v>
       </c>
@@ -20448,7 +20447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <v>25</v>
       </c>
@@ -20472,7 +20471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <v>26</v>
       </c>
@@ -20496,7 +20495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>27</v>
       </c>
@@ -20520,7 +20519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <v>28</v>
       </c>
@@ -20544,7 +20543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <v>29</v>
       </c>
@@ -20568,7 +20567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <v>30</v>
       </c>
@@ -20580,7 +20579,7 @@
       </c>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <v>31</v>
       </c>
@@ -20607,14 +20606,14 @@
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="G5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="1" t="s">
         <v>70</v>
       </c>
@@ -20628,7 +20627,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -20642,7 +20641,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -20662,7 +20661,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -20682,7 +20681,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -20702,7 +20701,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
@@ -20719,7 +20718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
@@ -20736,7 +20735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="1" t="s">
         <v>59</v>
       </c>
@@ -20753,7 +20752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
@@ -20770,7 +20769,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
@@ -20787,7 +20786,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
@@ -20804,7 +20803,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
@@ -20821,7 +20820,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
@@ -20835,7 +20834,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
@@ -20849,7 +20848,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1" t="s">
         <v>42</v>
       </c>
@@ -20866,7 +20865,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
@@ -20883,7 +20882,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="1" t="s">
         <v>44</v>
       </c>
@@ -20900,7 +20899,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
@@ -20920,7 +20919,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
@@ -20940,7 +20939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
@@ -20960,7 +20959,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
@@ -20980,7 +20979,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
@@ -21000,7 +20999,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -21017,7 +21016,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="1" t="s">
         <v>14</v>
       </c>
@@ -21034,7 +21033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="1" t="s">
         <v>15</v>
       </c>
@@ -21051,7 +21050,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
@@ -21071,7 +21070,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
@@ -21091,7 +21090,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
@@ -21111,7 +21110,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="1" t="s">
         <v>31</v>
       </c>
@@ -21131,7 +21130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
@@ -21151,7 +21150,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="1" t="s">
         <v>33</v>
       </c>
@@ -21171,7 +21170,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="1" t="s">
         <v>34</v>
       </c>
@@ -21191,7 +21190,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="1" t="s">
         <v>35</v>
       </c>
@@ -21225,17 +21224,17 @@
       <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.62890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.62890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.15625" customWidth="1"/>
+    <col min="10" max="10" width="8.7890625" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -21246,7 +21245,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -21263,7 +21262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>0</v>
       </c>
@@ -21286,7 +21285,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>0</v>
       </c>
@@ -21309,7 +21308,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>0</v>
       </c>
@@ -21332,7 +21331,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0</v>
       </c>
@@ -21355,7 +21354,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0</v>
       </c>
@@ -21381,7 +21380,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0</v>
       </c>
@@ -21416,7 +21415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0</v>
       </c>
@@ -21448,7 +21447,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0</v>
       </c>
@@ -21477,7 +21476,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0</v>
       </c>
@@ -21506,7 +21505,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0</v>
       </c>
@@ -21535,7 +21534,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>0</v>
       </c>
@@ -21564,7 +21563,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>0</v>
       </c>
@@ -21593,7 +21592,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>0</v>
       </c>
@@ -21619,7 +21618,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>0</v>
       </c>
@@ -21642,7 +21641,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>0</v>
       </c>
@@ -21665,7 +21664,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>0</v>
       </c>
@@ -21688,7 +21687,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -21717,7 +21716,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="5">
         <v>1</v>
       </c>
@@ -21743,7 +21742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="5">
         <v>1</v>
       </c>
@@ -21769,7 +21768,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="5">
         <v>1</v>
       </c>
@@ -21795,7 +21794,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="5">
         <v>1</v>
       </c>
@@ -21821,7 +21820,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="5">
         <v>1</v>
       </c>
@@ -21847,7 +21846,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="5">
         <v>1</v>
       </c>
@@ -21873,7 +21872,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="5">
         <v>1</v>
       </c>
@@ -21899,7 +21898,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="5">
         <v>1</v>
       </c>
@@ -21925,7 +21924,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="5">
         <v>1</v>
       </c>
@@ -21951,7 +21950,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="5">
         <v>1</v>
       </c>
@@ -21977,7 +21976,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="5">
         <v>1</v>
       </c>
@@ -22003,7 +22002,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="5">
         <v>1</v>
       </c>
@@ -22029,7 +22028,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="5">
         <v>1</v>
       </c>
@@ -22055,7 +22054,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="5">
         <v>1</v>
       </c>
@@ -22081,7 +22080,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="5">
         <v>1</v>
       </c>

</xml_diff>